<commit_message>
Task Board - few changes by Sourav
</commit_message>
<xml_diff>
--- a/Task Board - Team A - Sprint 3.xlsx
+++ b/Task Board - Team A - Sprint 3.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madvemul\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sourmaji\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="8250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sarthak Lav" sheetId="3" r:id="rId1"/>
-    <sheet name="Sourav Maji" sheetId="4" r:id="rId2"/>
+    <sheet name="Sourav Maji" sheetId="7" r:id="rId2"/>
     <sheet name="Madhuri Vemulapaty" sheetId="1" r:id="rId3"/>
-    <sheet name="Shreyash Pandey" sheetId="5" r:id="rId4"/>
-    <sheet name="Ankush Agrawal" sheetId="6" r:id="rId5"/>
+    <sheet name="Ankush Agrawal" sheetId="6" r:id="rId4"/>
+    <sheet name="Shreyash Pandey" sheetId="8" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="84">
   <si>
     <t>Agile Task Board</t>
   </si>
@@ -144,12 +144,6 @@
     <t>UI - Create Angular Component &amp; Template for "Delete Retailer Page" using Bootstrap &amp; Angular</t>
   </si>
   <si>
-    <t>UI - Create Angular Component &amp; Template for "Delete Return Page" using Bootstrap &amp; Angular</t>
-  </si>
-  <si>
-    <t>UI - Create Angular Component &amp; Template for "Edit Return Page" using Bootstrap &amp; Angular</t>
-  </si>
-  <si>
     <t>UI - Create Angular Component &amp; Template for "Place Return Page" using Bootstrap &amp; Angular</t>
   </si>
   <si>
@@ -159,12 +153,6 @@
     <t>UI - Create ReturnService using Angular for CRUD operations</t>
   </si>
   <si>
-    <t>Create SQL Server table named "Return" and "ReturnDetails"</t>
-  </si>
-  <si>
-    <t>Create Return</t>
-  </si>
-  <si>
     <t>Return and Cancel a Product</t>
   </si>
   <si>
@@ -216,9 +204,6 @@
     <t>Shreyash Pandey</t>
   </si>
   <si>
-    <t>UI - Create Angular Component &amp; Template for "Create Online Order Page" using Bootstrap &amp; Angular</t>
-  </si>
-  <si>
     <t>UI - Create Angular Component &amp; Template for "Order Page" using Bootstrap &amp; Angular</t>
   </si>
   <si>
@@ -235,6 +220,66 @@
   </si>
   <si>
     <t>Ankush Agrawal</t>
+  </si>
+  <si>
+    <t>Create SQL Server table named "ReturnDetails"</t>
+  </si>
+  <si>
+    <t>ReturnDetails</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          UI - Create Angular Component &amp; Template for "Cancel Order Page" using Bootstrap &amp; Angular </t>
+  </si>
+  <si>
+    <t>Create SQL Server table named "Return"</t>
+  </si>
+  <si>
+    <t>Order Return</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "Sales Person Order Report" using Bootstrap &amp; Angular</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "Retailer Order Report" using Bootstrap &amp; Angular</t>
+  </si>
+  <si>
+    <t>Create BL for "Report" as ReportBL</t>
+  </si>
+  <si>
+    <t>Create Report</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "Admin Login" using Bootstrap &amp; Angular</t>
+  </si>
+  <si>
+    <t>UI - Create AdminService using Angular for Retrive and Login operations</t>
+  </si>
+  <si>
+    <t>Create SQL Server table named "Admin"</t>
+  </si>
+  <si>
+    <t>issue with concept and silly mistakes in character casing</t>
+  </si>
+  <si>
+    <t>issue with fakedb, array handling and objects</t>
+  </si>
+  <si>
+    <t>character casing mistakes, array handling and objects</t>
+  </si>
+  <si>
+    <t>issue with fakedb, array handling, routing and objects</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "Create/Edit/Delete Online Order Page" using Bootstrap &amp; Angular</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "Order Details" using Bootstrap &amp; Angular</t>
+  </si>
+  <si>
+    <t>issue with concept and mistakes in character casing</t>
+  </si>
+  <si>
+    <t>UI - Create Angular Component &amp; Template for "View Return History" using Bootstrap &amp; Angular</t>
   </si>
 </sst>
 </file>
@@ -321,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -361,14 +406,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,7 +478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -481,7 +530,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -683,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -694,17 +743,18 @@
     <col min="1" max="1" width="95.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="19.7109375" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
@@ -712,7 +762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
@@ -720,7 +770,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -728,8 +778,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
@@ -740,59 +790,127 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="4:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D12:D18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -801,10 +919,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -812,33 +930,34 @@
     <col min="1" max="1" width="95.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="36" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -846,8 +965,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
@@ -858,59 +977,239 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2</v>
+      </c>
+      <c r="C14" s="9">
+        <v>2</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="9">
+        <v>3</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="20"/>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="18" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
         <v>38</v>
       </c>
+      <c r="B26" s="9">
+        <v>2</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="9">
+        <v>2</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D12:D17"/>
+    <mergeCell ref="D24:D29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -919,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -930,17 +1229,18 @@
     <col min="1" max="1" width="104.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="26" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -948,7 +1248,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -956,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -964,8 +1264,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -976,122 +1276,277 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>2</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="B15" s="2">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B23" s="2">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B26" s="9">
+        <v>2</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B27" s="2">
+        <v>2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="20"/>
+    </row>
+    <row r="30" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D30" s="20"/>
+    </row>
+    <row r="31" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="D23:D31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1101,10 +1556,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1112,33 +1567,34 @@
     <col min="1" max="1" width="95.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="31.85546875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1146,8 +1602,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
@@ -1158,97 +1614,111 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>2</v>
+      </c>
+      <c r="C9" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="9">
+        <v>3</v>
+      </c>
+      <c r="C11" s="9">
+        <v>4</v>
+      </c>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="B14" s="9">
+        <v>5</v>
+      </c>
+      <c r="C14" s="9">
+        <v>6</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+        <v>81</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D10:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1257,10 +1727,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1268,33 +1738,34 @@
     <col min="1" max="1" width="95.7109375" style="9" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="24.5703125" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="9"/>
+    <col min="4" max="4" width="25.85546875" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:4" s="7" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-    </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1302,8 +1773,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="7" customFormat="1" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>1</v>
       </c>
@@ -1314,55 +1785,269 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2</v>
+      </c>
+      <c r="C12" s="9">
+        <v>3</v>
+      </c>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <v>3</v>
+      </c>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="9">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
-    </row>
-    <row r="16" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="16"/>
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9">
+        <v>1</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="9">
+        <v>2</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2</v>
+      </c>
+      <c r="D23" s="20"/>
+    </row>
+    <row r="24" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2</v>
+      </c>
+      <c r="C24" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="D24" s="20"/>
+    </row>
+    <row r="25" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="D26" s="20"/>
+    </row>
+    <row r="27" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="20"/>
+    </row>
+    <row r="28" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D11:D17"/>
+    <mergeCell ref="D22:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>